<commit_message>
update: add timezone column
</commit_message>
<xml_diff>
--- a/resources/request.xlsx
+++ b/resources/request.xlsx
@@ -77,6 +77,9 @@
     <t>Aux_time_str</t>
   </si>
   <si>
+    <t>Timezone</t>
+  </si>
+  <si>
     <t>Parameter_avoid</t>
   </si>
   <si>
@@ -87,9 +90,6 @@
   </si>
   <si>
     <t>73_148_ES</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>tolls</t>
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -180,9 +180,6 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -489,24 +486,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="3" width="13.005" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="3" width="13.005" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="3" width="22.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="3" width="13.005" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="3" width="13.005" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="3" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -543,13 +541,16 @@
       <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="5">
         <v>19.556278</v>
@@ -569,15 +570,14 @@
         <v>4</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>